<commit_message>
Implement BERT into model
</commit_message>
<xml_diff>
--- a/PredictionChart.xlsx
+++ b/PredictionChart.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niko/Desktop/School/Spring Classes/Sp24/4650 (Natural Language)/CS4650Group3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5CB317-9CDF-4349-A820-55E181B3D863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9733F-9B72-844A-A91E-A6580205CEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-4320" windowWidth="68800" windowHeight="28800" xr2:uid="{BCBCAB86-CFD2-574A-A124-EF841336E079}"/>
+    <workbookView xWindow="63800" yWindow="-3820" windowWidth="34400" windowHeight="28300" xr2:uid="{BCBCAB86-CFD2-574A-A124-EF841336E079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$1:$AC$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$AC$2</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1256,16 +1238,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>671364</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>107359</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>635001</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6518</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>214165</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>3865</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>191449</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>102054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1612,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029F22B0-72E8-9941-93C8-C55D02DA482B}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="358" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="358" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>